<commit_message>
fixed matlab path error
</commit_message>
<xml_diff>
--- a/instances/Test.xlsx
+++ b/instances/Test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\aelle\SDP\mr-sos-sdp\instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\aelle\mr-sos-dp\instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01269554-DDF0-4C3C-B8ED-EBA6687B8834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200F87B5-3816-495A-AF44-15B2F5C0138E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>k</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Inst</t>
   </si>
@@ -51,16 +48,16 @@
     <t>GAP UB opt</t>
   </si>
   <si>
-    <t>GAP LB heut</t>
-  </si>
-  <si>
-    <t>GAP UB heu</t>
-  </si>
-  <si>
-    <t>It</t>
-  </si>
-  <si>
     <t>GAP LB-UB</t>
+  </si>
+  <si>
+    <t>GAP uB heut</t>
+  </si>
+  <si>
+    <t>GAP LB heu</t>
+  </si>
+  <si>
+    <t>Num it</t>
   </si>
 </sst>
 </file>
@@ -100,7 +97,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -378,57 +375,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added from file results
</commit_message>
<xml_diff>
--- a/instances/Test.xlsx
+++ b/instances/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\aelle\mr-sos-dp\instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F921CA-F57B-4472-BFC5-B914FA43CB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8351FF-378D-4432-A516-2619BB1B81A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,15 @@
     <sheet name="Resultsonlyray" sheetId="2" r:id="rId2"/>
     <sheet name="Random" sheetId="4" r:id="rId3"/>
     <sheet name="Combin" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
-    <sheet name="Foglio2" sheetId="3" r:id="rId6"/>
+    <sheet name="From file" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId6"/>
+    <sheet name="Foglio2" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Random!$A$1:$U$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$U$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Resultsonlyray!$A$1:$U$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet3!$G$2:$K$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet3!$G$2:$K$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="62">
   <si>
     <t>Inst</t>
   </si>
@@ -8515,7 +8516,7 @@
   <dimension ref="A1:U53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11992,11 +11993,759 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54CF4FC-39B9-4234-9B92-EE35ABBB41C2}">
+  <dimension ref="A1:U11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>12881.1</v>
+      </c>
+      <c r="E2">
+        <v>12881.1</v>
+      </c>
+      <c r="F2">
+        <v>12565.4</v>
+      </c>
+      <c r="G2">
+        <v>12881.1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>8</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>12</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>12881.1</v>
+      </c>
+      <c r="E3">
+        <v>12881.1</v>
+      </c>
+      <c r="F3">
+        <v>12604.6</v>
+      </c>
+      <c r="G3">
+        <v>12881.1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>16</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>23437.4</v>
+      </c>
+      <c r="E4">
+        <v>23437.4</v>
+      </c>
+      <c r="F4">
+        <v>22223.9</v>
+      </c>
+      <c r="G4">
+        <v>27783.3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>261</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>266</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>15327.4</v>
+      </c>
+      <c r="E5">
+        <v>15327.4</v>
+      </c>
+      <c r="F5">
+        <v>12915.3</v>
+      </c>
+      <c r="G5">
+        <v>16111.8</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>209</v>
+      </c>
+      <c r="O5">
+        <v>68</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>279</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>11455.6</v>
+      </c>
+      <c r="E6">
+        <v>11455.6</v>
+      </c>
+      <c r="F6">
+        <v>9399.0300000000007</v>
+      </c>
+      <c r="G6">
+        <v>13222.2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>212</v>
+      </c>
+      <c r="O6">
+        <v>80</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>295</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>6764.88</v>
+      </c>
+      <c r="E7">
+        <v>6764.88</v>
+      </c>
+      <c r="F7">
+        <v>5722.23</v>
+      </c>
+      <c r="G7">
+        <v>7583.65</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>221</v>
+      </c>
+      <c r="O7">
+        <v>58</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>281</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>5817.57</v>
+      </c>
+      <c r="E8">
+        <v>5818.87</v>
+      </c>
+      <c r="F8">
+        <v>4415.0200000000004</v>
+      </c>
+      <c r="G8">
+        <v>6491.47</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>252</v>
+      </c>
+      <c r="O8">
+        <v>25</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>279</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="T8" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>5006.1000000000004</v>
+      </c>
+      <c r="E9">
+        <v>5006.1000000000004</v>
+      </c>
+      <c r="F9">
+        <v>3531.99</v>
+      </c>
+      <c r="G9">
+        <v>5801.51</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>249</v>
+      </c>
+      <c r="O9">
+        <v>93</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>345</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>4376.1899999999996</v>
+      </c>
+      <c r="E10">
+        <v>4376.1899999999996</v>
+      </c>
+      <c r="F10">
+        <v>3093.63</v>
+      </c>
+      <c r="G10">
+        <v>4990.05</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>298</v>
+      </c>
+      <c r="O10">
+        <v>121</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>421</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="U10" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>3794.49</v>
+      </c>
+      <c r="E11">
+        <v>3878.58</v>
+      </c>
+      <c r="F11">
+        <v>2614.23</v>
+      </c>
+      <c r="G11">
+        <v>4341.71</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>241</v>
+      </c>
+      <c r="O11">
+        <v>78</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>320</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36821B76-D2B7-4422-9A90-FDAB2BADC397}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
@@ -13486,7 +14235,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C70EFDF-9142-43FB-B065-077FF2D5F0B9}">
   <dimension ref="A1:F18"/>
   <sheetViews>

</xml_diff>

<commit_message>
new test from file
</commit_message>
<xml_diff>
--- a/instances/Test.xlsx
+++ b/instances/Test.xlsx
@@ -8,25 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\aelle\mr-sos-dp\instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DDE6A7-52B1-4F13-A81D-8C96DF04CC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3031152F-FD0C-4DDD-B8F3-AA1778E35FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="Resultsonlyray" sheetId="2" r:id="rId2"/>
     <sheet name="Random" sheetId="4" r:id="rId3"/>
     <sheet name="Combin" sheetId="5" r:id="rId4"/>
-    <sheet name="From file" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="6" r:id="rId6"/>
-    <sheet name="Foglio2" sheetId="3" r:id="rId7"/>
+    <sheet name="Genetic" sheetId="7" r:id="rId5"/>
+    <sheet name="Anticlustering" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'From file'!$A$1:$U$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Genetic!$A$1:$U$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Random!$A$1:$U$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$U$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Resultsonlyray!$A$1:$U$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet3!$G$2:$K$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sheet3!$G$2:$K$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="73">
   <si>
     <t>Inst</t>
   </si>
@@ -196,60 +196,6 @@
     <t>gr666</t>
   </si>
   <si>
-    <t>RAY</t>
-  </si>
-  <si>
-    <t>IT+RAY</t>
-  </si>
-  <si>
-    <t>Diff</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>ruspini4</t>
-  </si>
-  <si>
-    <t>ch1502</t>
-  </si>
-  <si>
-    <t>ch1503</t>
-  </si>
-  <si>
-    <t>ch1504</t>
-  </si>
-  <si>
-    <t>ch1505</t>
-  </si>
-  <si>
-    <t>ch1506</t>
-  </si>
-  <si>
-    <t>ch1507</t>
-  </si>
-  <si>
-    <t>ch1508</t>
-  </si>
-  <si>
-    <t>ch1509</t>
-  </si>
-  <si>
-    <t>ch15010</t>
-  </si>
-  <si>
-    <t>d1987</t>
-  </si>
-  <si>
-    <t>d19815</t>
-  </si>
-  <si>
-    <t>gr2022</t>
-  </si>
-  <si>
-    <t>gr2023</t>
-  </si>
-  <si>
     <t>Random</t>
   </si>
   <si>
@@ -261,19 +207,96 @@
   <si>
     <t>ali535</t>
   </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/ruspini_2.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/ruspini_3.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/ruspini_4.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/ch150_2.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/ch150_3.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/ch150_4.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/gr202_2.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/gr202_3.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/gr202_4.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/pr299_2.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/pr299_3.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/pr299_4.txt</t>
+  </si>
+  <si>
+    <t># Clusters</t>
+  </si>
+  <si>
+    <t># Partitions</t>
+  </si>
+  <si>
+    <t>OPT</t>
+  </si>
+  <si>
+    <t>Type test</t>
+  </si>
+  <si>
+    <t>p from file</t>
+  </si>
+  <si>
+    <t>UB-LB GAP (%)</t>
+  </si>
+  <si>
+    <t>OPT_LB GAP (%)</t>
+  </si>
+  <si>
+    <t>OPT-LB GAP (%)</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/ali535_2.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/ali535_3.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/ali535_4.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/art_200_2.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/art_200_3.txt</t>
+  </si>
+  <si>
+    <t>../instances/anticlust/art_200_4.txt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,7 +313,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -298,44 +321,22 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -12000,9 +12001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54CF4FC-39B9-4234-9B92-EE35ABBB41C2}">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -12093,7 +12092,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -12158,7 +12157,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -12223,7 +12222,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -12288,7 +12287,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -12353,7 +12352,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -13983,6 +13982,1105 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C70EFDF-9142-43FB-B065-077FF2D5F0B9}">
+  <dimension ref="A1:M25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>12881.1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2">
+        <v>12247.5</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5">
+        <f>(D2-F2)/D2*100</f>
+        <v>4.9188345715816224</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2">
+        <v>12805.5</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="5">
+        <f>(D2-K2)/D2*100</f>
+        <v>0.58690639774553699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>12881.1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3">
+        <v>11180.2</v>
+      </c>
+      <c r="G3">
+        <v>13</v>
+      </c>
+      <c r="H3" s="5">
+        <f t="shared" ref="H3:H25" si="0">(D3-F3)/D3*100</f>
+        <v>13.204617618060565</v>
+      </c>
+      <c r="I3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3">
+        <v>12651</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3" s="5">
+        <f t="shared" ref="M3:M25" si="1">(D3-K3)/D3*100</f>
+        <v>1.7863381232969262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>12881.1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4">
+        <v>9361.61</v>
+      </c>
+      <c r="G4">
+        <v>27</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" si="0"/>
+        <v>27.322899441817857</v>
+      </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4">
+        <v>12478.2</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4" s="5">
+        <f t="shared" si="1"/>
+        <v>3.1278384610009988</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6772120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="3">
+        <v>6594960</v>
+      </c>
+      <c r="G5">
+        <v>18</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" si="0"/>
+        <v>2.6160197988222298</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="3">
+        <v>6763750</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
+        <f t="shared" si="1"/>
+        <v>0.12359497469034808</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>6772120</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="3">
+        <v>6555940</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" si="0"/>
+        <v>3.1922056903894198</v>
+      </c>
+      <c r="I6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="3">
+        <v>6752570</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <f t="shared" si="1"/>
+        <v>0.28868360277136257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>6772120</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="3">
+        <v>6560740</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="0"/>
+        <v>3.1213268518573209</v>
+      </c>
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" s="3">
+        <v>6756180</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <f t="shared" si="1"/>
+        <v>0.23537680962534627</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4388510</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3688680</v>
+      </c>
+      <c r="G8">
+        <v>33</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="0"/>
+        <v>15.946870350073258</v>
+      </c>
+      <c r="I8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="3">
+        <v>4366630</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8" s="5">
+        <f t="shared" si="1"/>
+        <v>0.49857468708058084</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>4388510</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="3">
+        <v>4025280</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="0"/>
+        <v>8.2768411146379979</v>
+      </c>
+      <c r="I9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="3">
+        <v>4367960</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9" s="5">
+        <f t="shared" si="1"/>
+        <v>0.46826827328637738</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4388510</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3801470</v>
+      </c>
+      <c r="G10">
+        <v>34</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="0"/>
+        <v>13.37674973966107</v>
+      </c>
+      <c r="I10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" s="3">
+        <v>4330730</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10" s="5">
+        <f t="shared" si="1"/>
+        <v>1.3166199917511867</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2816830</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2559140</v>
+      </c>
+      <c r="G11">
+        <v>19</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" si="0"/>
+        <v>9.1482269075521074</v>
+      </c>
+      <c r="I11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" t="s">
+        <v>50</v>
+      </c>
+      <c r="K11" s="3">
+        <v>2806750</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11" s="5">
+        <f t="shared" si="1"/>
+        <v>0.35784907147396189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2816830</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2634030</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="0"/>
+        <v>6.4895645104603394</v>
+      </c>
+      <c r="I12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" s="3">
+        <v>2799940</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12" s="5">
+        <f t="shared" si="1"/>
+        <v>0.59961020011857302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2816830</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2543960</v>
+      </c>
+      <c r="G13">
+        <v>21</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="0"/>
+        <v>9.6871305687599172</v>
+      </c>
+      <c r="I13" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" s="3">
+        <v>2778380</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13" s="5">
+        <f t="shared" si="1"/>
+        <v>1.365009602993436</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>23437.4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14">
+        <v>23306.9</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.55680237569013624</v>
+      </c>
+      <c r="I14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14">
+        <v>23427.3</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14" s="5">
+        <f t="shared" si="1"/>
+        <v>4.3093517199016024E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>15327.4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15">
+        <v>11935.6</v>
+      </c>
+      <c r="G15">
+        <v>31</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" si="0"/>
+        <v>22.128997742604742</v>
+      </c>
+      <c r="I15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15">
+        <v>13580.2</v>
+      </c>
+      <c r="L15">
+        <v>17</v>
+      </c>
+      <c r="M15" s="5">
+        <f t="shared" si="1"/>
+        <v>11.39919360100212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>11455.6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16">
+        <v>8076.64</v>
+      </c>
+      <c r="G16">
+        <v>42</v>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" si="0"/>
+        <v>29.496141625056737</v>
+      </c>
+      <c r="I16" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16">
+        <v>9819.81</v>
+      </c>
+      <c r="L16">
+        <v>18</v>
+      </c>
+      <c r="M16" s="5">
+        <f t="shared" si="1"/>
+        <v>14.279391738538363</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>400724000</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="3">
+        <v>395686000</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5">
+        <f t="shared" si="0"/>
+        <v>1.2572244237929349</v>
+      </c>
+      <c r="I17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" t="s">
+        <v>56</v>
+      </c>
+      <c r="K17" s="3">
+        <v>400607000</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17" s="5">
+        <f t="shared" si="1"/>
+        <v>2.9197153152793445E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3">
+        <v>277437000</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="3">
+        <v>270341000</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18" s="5">
+        <f t="shared" si="0"/>
+        <v>2.5576977836409704</v>
+      </c>
+      <c r="I18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="3">
+        <v>277233000</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18" s="5">
+        <f t="shared" si="1"/>
+        <v>7.3530206857773117E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" s="3">
+        <v>217262000</v>
+      </c>
+      <c r="E19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="3">
+        <v>187705000</v>
+      </c>
+      <c r="G19">
+        <v>31</v>
+      </c>
+      <c r="H19" s="5">
+        <f t="shared" si="0"/>
+        <v>13.604311844685219</v>
+      </c>
+      <c r="I19" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" t="s">
+        <v>58</v>
+      </c>
+      <c r="K19" s="3">
+        <v>216408000</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19" s="5">
+        <f t="shared" si="1"/>
+        <v>0.39307380029641631</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>990552</v>
+      </c>
+      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20">
+        <v>983578</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="5">
+        <f t="shared" si="0"/>
+        <v>0.70405188218286374</v>
+      </c>
+      <c r="I20" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" t="s">
+        <v>67</v>
+      </c>
+      <c r="K20">
+        <v>990482</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20" s="5">
+        <f t="shared" si="1"/>
+        <v>7.066766812847786E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>457631</v>
+      </c>
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21">
+        <v>447801</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" si="0"/>
+        <v>2.1480188186552049</v>
+      </c>
+      <c r="I21" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21">
+        <v>457463</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21" s="5">
+        <f t="shared" si="1"/>
+        <v>3.6710799749142868E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>320279</v>
+      </c>
+      <c r="E22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22">
+        <v>302879</v>
+      </c>
+      <c r="G22">
+        <v>14</v>
+      </c>
+      <c r="H22" s="5">
+        <f t="shared" si="0"/>
+        <v>5.4327633094895393</v>
+      </c>
+      <c r="I22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22">
+        <v>319517</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22" s="5">
+        <f t="shared" si="1"/>
+        <v>0.2379175656224729</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>298.47800000000001</v>
+      </c>
+      <c r="E23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23">
+        <v>292.93799999999999</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" si="0"/>
+        <v>1.8560831954113941</v>
+      </c>
+      <c r="I23" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" t="s">
+        <v>70</v>
+      </c>
+      <c r="K23">
+        <v>297.721</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23" s="5">
+        <f t="shared" si="1"/>
+        <v>0.25362003229718943</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>298.47800000000001</v>
+      </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24">
+        <v>280.01299999999998</v>
+      </c>
+      <c r="G24">
+        <v>7</v>
+      </c>
+      <c r="H24" s="5">
+        <f t="shared" si="0"/>
+        <v>6.1863855962583614</v>
+      </c>
+      <c r="I24" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" t="s">
+        <v>71</v>
+      </c>
+      <c r="K24">
+        <v>297.06099999999998</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24" s="5">
+        <f t="shared" si="1"/>
+        <v>0.47474185702129806</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>298.47800000000001</v>
+      </c>
+      <c r="E25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25">
+        <v>276.08699999999999</v>
+      </c>
+      <c r="G25">
+        <v>8</v>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" si="0"/>
+        <v>7.5017254202989898</v>
+      </c>
+      <c r="I25" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" t="s">
+        <v>72</v>
+      </c>
+      <c r="K25">
+        <v>297.59899999999999</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25" s="5">
+        <f t="shared" si="1"/>
+        <v>0.29449406656437627</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36821B76-D2B7-4422-9A90-FDAB2BADC397}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K50"/>
@@ -13994,10 +15092,10 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="8"/>
+      <c r="C1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -14007,10 +15105,10 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -14019,10 +15117,10 @@
         <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -15475,383 +16573,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C70EFDF-9142-43FB-B065-077FF2D5F0B9}">
-  <dimension ref="A1:F18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="7">
-        <f>VLOOKUP(C2,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.04</v>
-      </c>
-      <c r="E2" s="7">
-        <f>VLOOKUP(C2,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.04</v>
-      </c>
-      <c r="F2" s="2">
-        <f>D2-E2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="7">
-        <f>VLOOKUP(C3,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E3" s="7">
-        <f>VLOOKUP(C3,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.5</v>
-      </c>
-      <c r="F3" s="2">
-        <f t="shared" ref="F3:F16" si="0">D3-E3</f>
-        <v>-0.36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="7">
-        <f>VLOOKUP(C4,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.27</v>
-      </c>
-      <c r="E4" s="7">
-        <f>VLOOKUP(C4,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.11</v>
-      </c>
-      <c r="F4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.16000000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="7">
-        <f>VLOOKUP(C5,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.33</v>
-      </c>
-      <c r="E5" s="7">
-        <f>VLOOKUP(C5,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.24</v>
-      </c>
-      <c r="F5" s="2">
-        <f t="shared" si="0"/>
-        <v>9.0000000000000024E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="7">
-        <f>VLOOKUP(C6,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.17</v>
-      </c>
-      <c r="E6" s="7">
-        <f>VLOOKUP(C6,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.16</v>
-      </c>
-      <c r="F6" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0000000000000009E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="7">
-        <f>VLOOKUP(C7,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.33</v>
-      </c>
-      <c r="E7" s="7">
-        <f>VLOOKUP(C7,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.38</v>
-      </c>
-      <c r="F7" s="2">
-        <f t="shared" si="0"/>
-        <v>-4.9999999999999989E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="7">
-        <f>VLOOKUP(C8,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.42</v>
-      </c>
-      <c r="E8" s="7">
-        <f>VLOOKUP(C8,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.39</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="0"/>
-        <v>2.9999999999999971E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="7">
-        <f>VLOOKUP(C9,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.36</v>
-      </c>
-      <c r="E9" s="7">
-        <f>VLOOKUP(C9,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.4</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="0"/>
-        <v>-4.0000000000000036E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="7">
-        <f>VLOOKUP(C10,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.4</v>
-      </c>
-      <c r="E10" s="7">
-        <f>VLOOKUP(C10,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.33</v>
-      </c>
-      <c r="F10" s="2">
-        <f t="shared" si="0"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="7">
-        <f>VLOOKUP(C11,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.35</v>
-      </c>
-      <c r="E11" s="7">
-        <f>VLOOKUP(C11,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.36</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="0"/>
-        <v>-1.0000000000000009E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="7">
-        <f>VLOOKUP(C12,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.41</v>
-      </c>
-      <c r="E12" s="7">
-        <f>VLOOKUP(C12,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.37</v>
-      </c>
-      <c r="F12" s="2">
-        <f t="shared" si="0"/>
-        <v>3.999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="7">
-        <f>VLOOKUP(C13,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.5</v>
-      </c>
-      <c r="E13" s="7">
-        <f>VLOOKUP(C13,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.42</v>
-      </c>
-      <c r="F13" s="2">
-        <f t="shared" si="0"/>
-        <v>8.0000000000000016E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="7">
-        <f>VLOOKUP(C14,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.46</v>
-      </c>
-      <c r="E14" s="7">
-        <f>VLOOKUP(C14,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.51</v>
-      </c>
-      <c r="F14" s="2">
-        <f t="shared" si="0"/>
-        <v>-4.9999999999999989E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="7">
-        <f>VLOOKUP(C15,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E15" s="7">
-        <f>VLOOKUP(C15,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.22</v>
-      </c>
-      <c r="F15" s="2">
-        <f t="shared" si="0"/>
-        <v>-7.9999999999999988E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="7">
-        <f>VLOOKUP(C16,Results!$D$1:$V$16,16,FALSE)</f>
-        <v>0.35</v>
-      </c>
-      <c r="E16" s="7">
-        <f>VLOOKUP(C16,Resultsonlyray!$D$1:$V$52,16,FALSE)</f>
-        <v>0.3</v>
-      </c>
-      <c r="F16" s="2">
-        <f t="shared" si="0"/>
-        <v>4.9999999999999989E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update structure for efficiency
</commit_message>
<xml_diff>
--- a/instances/Test.xlsx
+++ b/instances/Test.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\aelle\mr-sos-dp\instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3031152F-FD0C-4DDD-B8F3-AA1778E35FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144E2D74-9182-4A30-8849-8A65A607BECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="Resultsonlyray" sheetId="2" r:id="rId2"/>
     <sheet name="Random" sheetId="4" r:id="rId3"/>
     <sheet name="Combin" sheetId="5" r:id="rId4"/>
-    <sheet name="Genetic" sheetId="7" r:id="rId5"/>
-    <sheet name="Anticlustering" sheetId="3" r:id="rId6"/>
-    <sheet name="Sheet3" sheetId="6" r:id="rId7"/>
+    <sheet name="Anticlustering" sheetId="3" r:id="rId5"/>
+    <sheet name="Genetic" sheetId="7" r:id="rId6"/>
+    <sheet name="Cluster-Part" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Genetic!$A$1:$U$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Genetic!$A$1:$U$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Random!$A$1:$U$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$U$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Resultsonlyray!$A$1:$U$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sheet3!$G$2:$K$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Sheet3!$G$2:$K$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="55">
   <si>
     <t>Inst</t>
   </si>
@@ -211,45 +212,6 @@
     <t>a</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/ruspini_2.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/ruspini_3.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/ruspini_4.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/ch150_2.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/ch150_3.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/ch150_4.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/gr202_2.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/gr202_3.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/gr202_4.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/pr299_2.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/pr299_3.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/pr299_4.txt</t>
-  </si>
-  <si>
     <t># Clusters</t>
   </si>
   <si>
@@ -262,9 +224,6 @@
     <t>Type test</t>
   </si>
   <si>
-    <t>p from file</t>
-  </si>
-  <si>
     <t>UB-LB GAP (%)</t>
   </si>
   <si>
@@ -274,22 +233,10 @@
     <t>OPT-LB GAP (%)</t>
   </si>
   <si>
-    <t>../instances/anticlust/ali535_2.txt</t>
+    <t>m</t>
   </si>
   <si>
-    <t>../instances/anticlust/ali535_3.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/ali535_4.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/art_200_2.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/art_200_3.txt</t>
-  </si>
-  <si>
-    <t>../instances/anticlust/art_200_4.txt</t>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -330,10 +277,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11998,6 +11945,723 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C70EFDF-9142-43FB-B065-077FF2D5F0B9}">
+  <dimension ref="A1:K43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>12881.1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2">
+        <v>12848.9</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2">
+        <v>12865.2</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>12881.1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3">
+        <v>12864.3</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3">
+        <v>12846.4</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>12881.1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4">
+        <v>12848.8</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4">
+        <v>12755.9</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6772120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="3">
+        <v>5276180</v>
+      </c>
+      <c r="G5">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="3">
+        <v>6761160</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>6772120</v>
+      </c>
+      <c r="E6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="3">
+        <v>6149850</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="3">
+        <v>6366870</v>
+      </c>
+      <c r="J6" s="3">
+        <v>6</v>
+      </c>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>6772120</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="3">
+        <v>6259170</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="3">
+        <v>6332250</v>
+      </c>
+      <c r="J7" s="3">
+        <v>6</v>
+      </c>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4388510</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3679570</v>
+      </c>
+      <c r="G8">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="3">
+        <v>3842980</v>
+      </c>
+      <c r="J8" s="3">
+        <v>12</v>
+      </c>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>4388510</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3710000</v>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="3">
+        <v>4018200</v>
+      </c>
+      <c r="J9" s="3">
+        <v>8</v>
+      </c>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4388510</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3969110</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="3">
+        <v>3842550</v>
+      </c>
+      <c r="J10" s="3">
+        <v>12</v>
+      </c>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2816830</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2711840</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2727570</v>
+      </c>
+      <c r="J11" s="3">
+        <v>3</v>
+      </c>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2816830</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2739630</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2705530</v>
+      </c>
+      <c r="J12" s="3">
+        <v>4</v>
+      </c>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2816830</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2707920</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="3">
+        <v>2730720</v>
+      </c>
+      <c r="J13" s="3">
+        <v>3</v>
+      </c>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>23437.4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14">
+        <v>19997.900000000001</v>
+      </c>
+      <c r="G14">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14">
+        <v>19963</v>
+      </c>
+      <c r="J14">
+        <v>15</v>
+      </c>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>15327.4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15">
+        <v>12355.6</v>
+      </c>
+      <c r="G15">
+        <v>19</v>
+      </c>
+      <c r="H15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15">
+        <v>12200.4</v>
+      </c>
+      <c r="J15">
+        <v>20</v>
+      </c>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>11455.6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16">
+        <v>8211.16</v>
+      </c>
+      <c r="G16">
+        <v>28</v>
+      </c>
+      <c r="H16" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16">
+        <v>8770.9</v>
+      </c>
+      <c r="J16">
+        <v>23</v>
+      </c>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>400724000</v>
+      </c>
+      <c r="E17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="3">
+        <v>400617000</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="3">
+        <v>400643000</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3">
+        <v>277437000</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="3">
+        <v>271692000</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="3">
+        <v>275739000</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1</v>
+      </c>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" s="3">
+        <v>217262000</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="3">
+        <v>195041000</v>
+      </c>
+      <c r="G19">
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="3">
+        <v>203480000</v>
+      </c>
+      <c r="J19" s="3">
+        <v>6</v>
+      </c>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K25" s="4"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D35" s="3"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D37" s="3"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D42" s="3"/>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D43" s="3"/>
+      <c r="F43" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54CF4FC-39B9-4234-9B92-EE35ABBB41C2}">
   <dimension ref="A1:U30"/>
   <sheetViews>
@@ -13981,11 +14645,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C70EFDF-9142-43FB-B065-077FF2D5F0B9}">
-  <dimension ref="A1:M25"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D4473C-2B3F-45DB-8781-28B54CB9D975}">
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -13993,57 +14657,37 @@
     <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
         <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -14057,36 +14701,19 @@
         <v>12881.1</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F2">
-        <v>12247.5</v>
+        <v>12791.8</v>
       </c>
       <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2" s="5">
-        <f>(D2-F2)/D2*100</f>
-        <v>4.9188345715816224</v>
-      </c>
-      <c r="I2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2">
-        <v>12805.5</v>
-      </c>
-      <c r="L2">
         <v>1</v>
       </c>
-      <c r="M2" s="5">
-        <f>(D2-K2)/D2*100</f>
-        <v>0.58690639774553699</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -14100,36 +14727,19 @@
         <v>12881.1</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F3">
-        <v>11180.2</v>
+        <v>12618.4</v>
       </c>
       <c r="G3">
-        <v>13</v>
-      </c>
-      <c r="H3" s="5">
-        <f t="shared" ref="H3:H25" si="0">(D3-F3)/D3*100</f>
-        <v>13.204617618060565</v>
-      </c>
-      <c r="I3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3">
-        <v>12651</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-      <c r="M3" s="5">
-        <f t="shared" ref="M3:M25" si="1">(D3-K3)/D3*100</f>
-        <v>1.7863381232969262</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -14143,36 +14753,19 @@
         <v>12881.1</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F4">
-        <v>9361.61</v>
+        <v>12522.8</v>
       </c>
       <c r="G4">
-        <v>27</v>
-      </c>
-      <c r="H4" s="5">
-        <f t="shared" si="0"/>
-        <v>27.322899441817857</v>
-      </c>
-      <c r="I4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K4">
-        <v>12478.2</v>
-      </c>
-      <c r="L4">
-        <v>3</v>
-      </c>
-      <c r="M4" s="5">
-        <f t="shared" si="1"/>
-        <v>3.1278384610009988</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -14186,36 +14779,19 @@
         <v>6772120</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3">
-        <v>6594960</v>
+        <v>6763440</v>
       </c>
       <c r="G5">
-        <v>18</v>
-      </c>
-      <c r="H5" s="5">
-        <f t="shared" si="0"/>
-        <v>2.6160197988222298</v>
-      </c>
-      <c r="I5" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" s="3">
-        <v>6763750</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5" s="5">
-        <f t="shared" si="1"/>
-        <v>0.12359497469034808</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -14229,36 +14805,19 @@
         <v>6772120</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F6" s="3">
-        <v>6555940</v>
+        <v>6716020</v>
       </c>
       <c r="G6">
-        <v>20</v>
-      </c>
-      <c r="H6" s="5">
-        <f t="shared" si="0"/>
-        <v>3.1922056903894198</v>
-      </c>
-      <c r="I6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" t="s">
-        <v>51</v>
-      </c>
-      <c r="K6" s="3">
-        <v>6752570</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="5">
-        <f t="shared" si="1"/>
-        <v>0.28868360277136257</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -14272,36 +14831,19 @@
         <v>6772120</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F7" s="3">
-        <v>6560740</v>
+        <v>6563300</v>
       </c>
       <c r="G7">
-        <v>7</v>
-      </c>
-      <c r="H7" s="5">
-        <f t="shared" si="0"/>
-        <v>3.1213268518573209</v>
-      </c>
-      <c r="I7" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" t="s">
-        <v>52</v>
-      </c>
-      <c r="K7" s="3">
-        <v>6756180</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7" s="5">
-        <f t="shared" si="1"/>
-        <v>0.23537680962534627</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -14315,36 +14857,19 @@
         <v>4388510</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F8" s="3">
-        <v>3688680</v>
+        <v>4249400</v>
       </c>
       <c r="G8">
-        <v>33</v>
-      </c>
-      <c r="H8" s="5">
-        <f t="shared" si="0"/>
-        <v>15.946870350073258</v>
-      </c>
-      <c r="I8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K8" s="3">
-        <v>4366630</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8" s="5">
-        <f t="shared" si="1"/>
-        <v>0.49857468708058084</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -14358,36 +14883,19 @@
         <v>4388510</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F9" s="3">
-        <v>4025280</v>
+        <v>4083740</v>
       </c>
       <c r="G9">
-        <v>20</v>
-      </c>
-      <c r="H9" s="5">
-        <f t="shared" si="0"/>
-        <v>8.2768411146379979</v>
-      </c>
-      <c r="I9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K9" s="3">
-        <v>4367960</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9" s="5">
-        <f t="shared" si="1"/>
-        <v>0.46826827328637738</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -14401,36 +14909,19 @@
         <v>4388510</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F10" s="3">
-        <v>3801470</v>
+        <v>4121730</v>
       </c>
       <c r="G10">
-        <v>34</v>
-      </c>
-      <c r="H10" s="5">
-        <f t="shared" si="0"/>
-        <v>13.37674973966107</v>
-      </c>
-      <c r="I10" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" t="s">
-        <v>52</v>
-      </c>
-      <c r="K10" s="3">
-        <v>4330730</v>
-      </c>
-      <c r="L10">
-        <v>2</v>
-      </c>
-      <c r="M10" s="5">
-        <f t="shared" si="1"/>
-        <v>1.3166199917511867</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -14444,36 +14935,19 @@
         <v>2816830</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F11" s="3">
-        <v>2559140</v>
+        <v>2750100</v>
       </c>
       <c r="G11">
-        <v>19</v>
-      </c>
-      <c r="H11" s="5">
-        <f t="shared" si="0"/>
-        <v>9.1482269075521074</v>
-      </c>
-      <c r="I11" t="s">
-        <v>46</v>
-      </c>
-      <c r="J11" t="s">
-        <v>50</v>
-      </c>
-      <c r="K11" s="3">
-        <v>2806750</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11" s="5">
-        <f t="shared" si="1"/>
-        <v>0.35784907147396189</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -14487,36 +14961,19 @@
         <v>2816830</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F12" s="3">
-        <v>2634030</v>
+        <v>2734800</v>
       </c>
       <c r="G12">
-        <v>9</v>
-      </c>
-      <c r="H12" s="5">
-        <f t="shared" si="0"/>
-        <v>6.4895645104603394</v>
-      </c>
-      <c r="I12" t="s">
-        <v>46</v>
-      </c>
-      <c r="J12" t="s">
-        <v>51</v>
-      </c>
-      <c r="K12" s="3">
-        <v>2799940</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12" s="5">
-        <f t="shared" si="1"/>
-        <v>0.59961020011857302</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -14530,36 +14987,19 @@
         <v>2816830</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F13" s="3">
-        <v>2543960</v>
+        <v>2636700</v>
       </c>
       <c r="G13">
-        <v>21</v>
-      </c>
-      <c r="H13" s="5">
-        <f t="shared" si="0"/>
-        <v>9.6871305687599172</v>
-      </c>
-      <c r="I13" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13" t="s">
-        <v>52</v>
-      </c>
-      <c r="K13" s="3">
-        <v>2778380</v>
-      </c>
-      <c r="L13">
-        <v>2</v>
-      </c>
-      <c r="M13" s="5">
-        <f t="shared" si="1"/>
-        <v>1.365009602993436</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -14573,36 +15013,19 @@
         <v>23437.4</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F14">
-        <v>23306.9</v>
+        <v>23357.8</v>
       </c>
       <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
         <v>1</v>
       </c>
-      <c r="H14" s="5">
-        <f t="shared" si="0"/>
-        <v>0.55680237569013624</v>
-      </c>
-      <c r="I14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J14" t="s">
-        <v>53</v>
-      </c>
-      <c r="K14">
-        <v>23427.3</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14" s="5">
-        <f t="shared" si="1"/>
-        <v>4.3093517199016024E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -14616,36 +15039,19 @@
         <v>15327.4</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F15">
-        <v>11935.6</v>
+        <v>12905.3</v>
       </c>
       <c r="G15">
-        <v>31</v>
-      </c>
-      <c r="H15" s="5">
-        <f t="shared" si="0"/>
-        <v>22.128997742604742</v>
-      </c>
-      <c r="I15" t="s">
-        <v>46</v>
-      </c>
-      <c r="J15" t="s">
-        <v>54</v>
-      </c>
-      <c r="K15">
-        <v>13580.2</v>
-      </c>
-      <c r="L15">
-        <v>17</v>
-      </c>
-      <c r="M15" s="5">
-        <f t="shared" si="1"/>
-        <v>11.39919360100212</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="H15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -14659,36 +15065,19 @@
         <v>11455.6</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F16">
-        <v>8076.64</v>
+        <v>9277.93</v>
       </c>
       <c r="G16">
-        <v>42</v>
-      </c>
-      <c r="H16" s="5">
-        <f t="shared" si="0"/>
-        <v>29.496141625056737</v>
-      </c>
-      <c r="I16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J16" t="s">
-        <v>55</v>
-      </c>
-      <c r="K16">
-        <v>9819.81</v>
-      </c>
-      <c r="L16">
-        <v>18</v>
-      </c>
-      <c r="M16" s="5">
-        <f t="shared" si="1"/>
-        <v>14.279391738538363</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="H16">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -14702,36 +15091,19 @@
         <v>400724000</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F17" s="3">
-        <v>395686000</v>
+        <v>400674000</v>
       </c>
       <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" s="5">
-        <f t="shared" si="0"/>
-        <v>1.2572244237929349</v>
-      </c>
-      <c r="I17" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" t="s">
-        <v>56</v>
-      </c>
-      <c r="K17" s="3">
-        <v>400607000</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17" s="5">
-        <f t="shared" si="1"/>
-        <v>2.9197153152793445E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -14745,36 +15117,19 @@
         <v>277437000</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F18" s="3">
-        <v>270341000</v>
+        <v>276955000</v>
       </c>
       <c r="G18">
-        <v>3</v>
-      </c>
-      <c r="H18" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5576977836409704</v>
-      </c>
-      <c r="I18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J18" t="s">
-        <v>57</v>
-      </c>
-      <c r="K18" s="3">
-        <v>277233000</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18" s="5">
-        <f t="shared" si="1"/>
-        <v>7.3530206857773117E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -14788,36 +15143,19 @@
         <v>217262000</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F19" s="3">
-        <v>187705000</v>
+        <v>213079000</v>
       </c>
       <c r="G19">
-        <v>31</v>
-      </c>
-      <c r="H19" s="5">
-        <f t="shared" si="0"/>
-        <v>13.604311844685219</v>
-      </c>
-      <c r="I19" t="s">
-        <v>46</v>
-      </c>
-      <c r="J19" t="s">
-        <v>58</v>
-      </c>
-      <c r="K19" s="3">
-        <v>216408000</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19" s="5">
-        <f t="shared" si="1"/>
-        <v>0.39307380029641631</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -14831,36 +15169,19 @@
         <v>990552</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F20">
-        <v>983578</v>
+        <v>990187</v>
       </c>
       <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20" s="5">
-        <f t="shared" si="0"/>
-        <v>0.70405188218286374</v>
-      </c>
-      <c r="I20" t="s">
-        <v>46</v>
-      </c>
-      <c r="J20" t="s">
-        <v>67</v>
-      </c>
-      <c r="K20">
-        <v>990482</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20" s="5">
-        <f t="shared" si="1"/>
-        <v>7.066766812847786E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -14874,36 +15195,19 @@
         <v>457631</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F21">
-        <v>447801</v>
+        <v>456096</v>
       </c>
       <c r="G21">
-        <v>2</v>
-      </c>
-      <c r="H21" s="5">
-        <f t="shared" si="0"/>
-        <v>2.1480188186552049</v>
-      </c>
-      <c r="I21" t="s">
-        <v>46</v>
-      </c>
-      <c r="J21" t="s">
-        <v>68</v>
-      </c>
-      <c r="K21">
-        <v>457463</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21" s="5">
-        <f t="shared" si="1"/>
-        <v>3.6710799749142868E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -14917,36 +15221,19 @@
         <v>320279</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F22">
-        <v>302879</v>
+        <v>317069</v>
       </c>
       <c r="G22">
-        <v>14</v>
-      </c>
-      <c r="H22" s="5">
-        <f t="shared" si="0"/>
-        <v>5.4327633094895393</v>
-      </c>
-      <c r="I22" t="s">
-        <v>46</v>
-      </c>
-      <c r="J22" t="s">
-        <v>69</v>
-      </c>
-      <c r="K22">
-        <v>319517</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22" s="5">
-        <f t="shared" si="1"/>
-        <v>0.2379175656224729</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -14960,36 +15247,19 @@
         <v>298.47800000000001</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F23">
-        <v>292.93799999999999</v>
+        <v>294.76799999999997</v>
       </c>
       <c r="G23">
-        <v>2</v>
-      </c>
-      <c r="H23" s="5">
-        <f t="shared" si="0"/>
-        <v>1.8560831954113941</v>
-      </c>
-      <c r="I23" t="s">
-        <v>46</v>
-      </c>
-      <c r="J23" t="s">
-        <v>70</v>
-      </c>
-      <c r="K23">
-        <v>297.721</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23" s="5">
-        <f t="shared" si="1"/>
-        <v>0.25362003229718943</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -15003,36 +15273,19 @@
         <v>298.47800000000001</v>
       </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F24">
-        <v>280.01299999999998</v>
+        <v>297.03699999999998</v>
       </c>
       <c r="G24">
-        <v>7</v>
-      </c>
-      <c r="H24" s="5">
-        <f t="shared" si="0"/>
-        <v>6.1863855962583614</v>
-      </c>
-      <c r="I24" t="s">
-        <v>46</v>
-      </c>
-      <c r="J24" t="s">
-        <v>71</v>
-      </c>
-      <c r="K24">
-        <v>297.06099999999998</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24" s="5">
-        <f t="shared" si="1"/>
-        <v>0.47474185702129806</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -15046,33 +15299,16 @@
         <v>298.47800000000001</v>
       </c>
       <c r="E25" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F25">
-        <v>276.08699999999999</v>
+        <v>294.50400000000002</v>
       </c>
       <c r="G25">
-        <v>8</v>
-      </c>
-      <c r="H25" s="5">
-        <f t="shared" si="0"/>
-        <v>7.5017254202989898</v>
-      </c>
-      <c r="I25" t="s">
-        <v>46</v>
-      </c>
-      <c r="J25" t="s">
-        <v>72</v>
-      </c>
-      <c r="K25">
-        <v>297.59899999999999</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25" s="5">
-        <f t="shared" si="1"/>
-        <v>0.29449406656437627</v>
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -15080,22 +15316,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36821B76-D2B7-4422-9A90-FDAB2BADC397}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">

</xml_diff>